<commit_message>
Menu para administrador y para usuario
</commit_message>
<xml_diff>
--- a/Tickets.xlsx
+++ b/Tickets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Flutter\tickets_web_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC09F28-48AD-45EF-9839-BF5A07FDA499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E630D6-2CA1-45F8-8D2E-4BC144A8F6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C0FA381-D708-4478-922F-AE5A18698AE2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>EMPRESAS</t>
   </si>
@@ -156,6 +156,69 @@
   </si>
   <si>
     <t>No poder desactivarse/borrarse a uno mismo</t>
+  </si>
+  <si>
+    <t>CABECERA TICKETS</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Fecha Creación</t>
+  </si>
+  <si>
+    <t>Usuario Creación</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Título</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>ESTADOS TICKETS</t>
+  </si>
+  <si>
+    <t>Borrador</t>
+  </si>
+  <si>
+    <t>Enviado</t>
+  </si>
+  <si>
+    <t>Rechazado</t>
+  </si>
+  <si>
+    <t>Devuelto Incompleto</t>
+  </si>
+  <si>
+    <t>Resuelto</t>
+  </si>
+  <si>
+    <t>Fecha Estado</t>
+  </si>
+  <si>
+    <t>Usuario Estado</t>
+  </si>
+  <si>
+    <t>DETALLE TICKETS</t>
+  </si>
+  <si>
+    <t>IdCabecera</t>
+  </si>
+  <si>
+    <t>Imagen</t>
+  </si>
+  <si>
+    <t>Comentario</t>
+  </si>
+  <si>
+    <t>Fecha</t>
   </si>
 </sst>
 </file>
@@ -549,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC422C99-E1B2-42BC-9FEB-41DADA2E2C18}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -565,7 +628,7 @@
     <col min="6" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -575,8 +638,14 @@
       <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -586,8 +655,14 @@
       <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -597,8 +672,14 @@
       <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -608,8 +689,14 @@
       <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -619,8 +706,14 @@
       <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -630,8 +723,14 @@
       <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -641,8 +740,11 @@
       <c r="F7" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -652,16 +754,22 @@
       <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I9" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -671,8 +779,11 @@
       <c r="E10" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I10" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -683,7 +794,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -694,7 +805,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -705,7 +816,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -716,7 +827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
@@ -724,12 +835,48 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C16" s="3" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I19" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I25" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Grabar Ticket con detalle
</commit_message>
<xml_diff>
--- a/Tickets.xlsx
+++ b/Tickets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Flutter\tickets_web_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D002F1FF-BD45-4B63-96F0-E6C755A84CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFBC022-21D2-49BE-916F-43B42FC3E4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2C0FA381-D708-4478-922F-AE5A18698AE2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C0FA381-D708-4478-922F-AE5A18698AE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="105">
   <si>
     <t>EMPRESAS</t>
   </si>
@@ -162,33 +162,18 @@
     <t>Id</t>
   </si>
   <si>
-    <t>ESTADOS TICKETS</t>
-  </si>
-  <si>
-    <t>Borrador</t>
-  </si>
-  <si>
     <t>Enviado</t>
   </si>
   <si>
-    <t>Rechazado</t>
-  </si>
-  <si>
     <t>Resuelto</t>
   </si>
   <si>
-    <t>Anulado</t>
-  </si>
-  <si>
     <t>Devuelto</t>
   </si>
   <si>
     <t>Tarea</t>
   </si>
   <si>
-    <t>SuperAdmin</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -213,9 +198,6 @@
     <t>Alta de User con envío de Email</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Editar SuperAdmin</t>
   </si>
   <si>
@@ -346,6 +328,52 @@
   </si>
   <si>
     <t>Alta de AdminKP con envío de Email</t>
+  </si>
+  <si>
+    <t>X lo mantenemos por las dudas</t>
+  </si>
+  <si>
+    <t>EnCursoDate</t>
+  </si>
+  <si>
+    <t>AdminKP</t>
+  </si>
+  <si>
+    <t>Asignado</t>
+  </si>
+  <si>
+    <t>En curso</t>
+  </si>
+  <si>
+    <t>ESTADOS TICKETS QUE PUEDE PONER CADA TIPO DE USUARIO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ESTADOS TICKETS QUE PUEDE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>VER</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> CADA TIPO DE USUARIO</t>
+    </r>
+  </si>
+  <si>
+    <t>AsignadoDate</t>
   </si>
 </sst>
 </file>
@@ -477,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -492,7 +520,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -504,9 +537,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC422C99-E1B2-42BC-9FEB-41DADA2E2C18}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9:N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -857,18 +891,20 @@
     <col min="5" max="5" width="3" style="1" customWidth="1"/>
     <col min="6" max="6" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" style="1"/>
-    <col min="11" max="11" width="1.77734375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" style="1"/>
+    <col min="8" max="8" width="14.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="2.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="1.77734375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" style="1"/>
     <col min="15" max="15" width="1.77734375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.5546875" style="1"/>
+    <col min="16" max="16" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.77734375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -878,23 +914,26 @@
       <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>71</v>
+      <c r="H1" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>103</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -904,12 +943,6 @@
       <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="L2" s="1" t="s">
         <v>40</v>
       </c>
@@ -919,8 +952,11 @@
       <c r="P2" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -930,23 +966,26 @@
       <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>72</v>
+      <c r="H3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -956,23 +995,26 @@
       <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>73</v>
+      <c r="H4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -982,23 +1024,24 @@
       <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>74</v>
+      <c r="H5" s="16"/>
+      <c r="J5" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1008,23 +1051,26 @@
       <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="15" t="s">
         <v>45</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1034,23 +1080,23 @@
       <c r="F7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>76</v>
+      <c r="H7" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1060,37 +1106,49 @@
       <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>77</v>
+      <c r="H8" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>78</v>
+      <c r="H9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1100,14 +1158,21 @@
       <c r="E10" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="H10" s="16"/>
       <c r="J10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N10" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1117,17 +1182,20 @@
       <c r="F11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="H11" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1137,8 +1205,14 @@
       <c r="F12" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -1148,14 +1222,23 @@
       <c r="F13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="H13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P13" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -1165,11 +1248,17 @@
       <c r="F14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H14" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
@@ -1177,16 +1266,53 @@
         <v>33</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="L16" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J19" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J20" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J26" s="16"/>
+    </row>
+    <row r="27" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J27" s="16"/>
+    </row>
+    <row r="28" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J28" s="16"/>
+    </row>
+    <row r="29" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J30" s="16"/>
+    </row>
+    <row r="32" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J32" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1196,11 +1322,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C40B2EA-A404-4D76-ACF6-3DCE9418AA55}">
-  <dimension ref="A1:D314"/>
+  <dimension ref="A1:E314"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:B17"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1210,220 +1336,229 @@
     <col min="5" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>55</v>
-      </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="B5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="B6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>52</v>
+      <c r="B7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>52</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="6" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>52</v>
       </c>
+      <c r="B10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>52</v>
+      <c r="E10" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>52</v>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>52</v>
+      <c r="B13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>52</v>
+      <c r="E13" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>52</v>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>64</v>
-      </c>
       <c r="C17" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -1434,59 +1569,57 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>52</v>
+      <c r="B21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>52</v>
+      <c r="B22" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>52</v>
+      <c r="B23" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="B24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
@@ -1495,139 +1628,139 @@
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>52</v>
+      <c r="B27" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>52</v>
+      <c r="B28" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>52</v>
+      <c r="B29" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>52</v>
+      <c r="B30" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>52</v>
+      <c r="B31" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>52</v>
+      <c r="B32" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>52</v>
+      <c r="B33" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>52</v>
+      <c r="B34" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>52</v>
+      <c r="B35" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>52</v>
+      <c r="B36" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>52</v>
+      <c r="B37" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="13" t="s">
-        <v>52</v>
+      <c r="B38" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>52</v>
+      <c r="B39" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -1639,35 +1772,35 @@
       <c r="D40" s="6"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="11"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="14"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>